<commit_message>
bj: update oncho forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Benin/stop/2024/bj_oncho_stop_2_2408_questions.xlsx
+++ b/ONCHO/Impact Assessments/Benin/stop/2024/bj_oncho_stop_2_2408_questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Benin\stop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Benin\stop\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC669D93-882F-4FF4-B753-89E6C9C30E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B19909D-2A4F-450E-B58C-387DF0C958C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="175">
   <si>
     <t>form_title</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Sélectionner un arrondissement</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
     <t>barcode</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>select_one yes_no_nk_rf</t>
   </si>
   <si>
-    <t>2) Sélectionner un village</t>
-  </si>
-  <si>
     <t>4) Numéro de maison</t>
   </si>
   <si>
@@ -278,9 +272,6 @@
     <t>p_consent</t>
   </si>
   <si>
-    <t>p_inf_gen</t>
-  </si>
-  <si>
     <t>p_num_maison</t>
   </si>
   <si>
@@ -326,12 +317,6 @@
     <t>${p_consent} = 'Oui' and ${p_took_ivm} != 'Non' and ${p_took_ivm} != 'Ne sait pas' and ${p_took_ivm} != 'Refuse de repondre'</t>
   </si>
   <si>
-    <t>${p_region} = region_list</t>
-  </si>
-  <si>
-    <t>${p_District} = district_list</t>
-  </si>
-  <si>
     <t>Scanner</t>
   </si>
   <si>
@@ -518,17 +503,74 @@
     <t>. &gt; 15</t>
   </si>
   <si>
-    <t>bj_oncho_stop_2_202306_questions_v3</t>
-  </si>
-  <si>
-    <t>(2023 Juillet) ONCHO Stop TDM - 2. Questionnaire individuel V3</t>
+    <t>(2024 Août) ONCHO Stop TDM - 2. Questionnaire individuel</t>
+  </si>
+  <si>
+    <t>bj_oncho_stop_2_2408_questions</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>join(' ', ${p_code_id})</t>
+  </si>
+  <si>
+    <t>begin repeat</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>position(..)</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>if (${C2} = 1,'',substring-after(${C1},${p_code_id}))</t>
+  </si>
+  <si>
+    <t>bj_o_p_2408</t>
+  </si>
+  <si>
+    <t>p_code_id</t>
+  </si>
+  <si>
+    <t>Numéro d'identification enregistré</t>
+  </si>
+  <si>
+    <t>if(${p_id_type} = 'Scanner', concat(${p_barecode_id}), concat(${p_manual_id}))</t>
+  </si>
+  <si>
+    <t>read_only</t>
+  </si>
+  <si>
+    <t>end repeat</t>
+  </si>
+  <si>
+    <t>not(selected(${C3}, ${p_code_id}))</t>
+  </si>
+  <si>
+    <t>Vous avez déjà utiliser cette identifiant</t>
+  </si>
+  <si>
+    <t>2.a Sélectionner un village</t>
+  </si>
+  <si>
+    <t>p_site_id</t>
+  </si>
+  <si>
+    <t>2.b. Sélectionner le code du village</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -595,8 +637,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -615,8 +663,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -639,13 +699,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -723,6 +813,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1013,13 +1136,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1032,13 +1155,13 @@
     <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.5" customWidth="1"/>
     <col min="8" max="8" width="34.25" customWidth="1"/>
-    <col min="9" max="9" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
     <col min="10" max="10" width="9.75" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.875" customWidth="1"/>
     <col min="12" max="12" width="36.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
@@ -1075,13 +1198,16 @@
       <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>15</v>
@@ -1104,12 +1230,12 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>27</v>
@@ -1126,12 +1252,12 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>33</v>
@@ -1146,19 +1272,17 @@
         <v>24</v>
       </c>
       <c r="K4" s="10"/>
-      <c r="L4" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>48</v>
+        <v>172</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="12"/>
@@ -1170,166 +1294,151 @@
         <v>24</v>
       </c>
       <c r="K5" s="10"/>
-      <c r="L5" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>38</v>
+        <v>174</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="10"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="10"/>
       <c r="J6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+    </row>
+    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="O9" s="30"/>
+    </row>
+    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="35"/>
+    </row>
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="35"/>
+    </row>
+    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="B12" s="16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
       <c r="F12" s="6"/>
       <c r="G12" s="13"/>
       <c r="H12" s="22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="6" t="s">
@@ -1338,22 +1447,22 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
       <c r="G13" s="13"/>
       <c r="H13" s="22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="6" t="s">
@@ -1362,22 +1471,22 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>135</v>
+        <v>34</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
       <c r="F14" s="6"/>
       <c r="G14" s="13"/>
       <c r="H14" s="22" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="6" t="s">
@@ -1386,22 +1495,22 @@
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
       <c r="G15" s="13"/>
       <c r="H15" s="22" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="6" t="s">
@@ -1410,48 +1519,51 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="F16" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J16" s="6"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
-    </row>
-    <row r="17" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="M16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="6" t="s">
-        <v>158</v>
-      </c>
+      <c r="F17" s="6"/>
       <c r="G17" s="13"/>
       <c r="H17" s="22" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="6" t="s">
@@ -1460,22 +1572,22 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
     </row>
-    <row r="18" spans="1:12" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
       <c r="F18" s="6"/>
       <c r="G18" s="13"/>
       <c r="H18" s="22" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="6" t="s">
@@ -1484,22 +1596,22 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
     </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
       <c r="G19" s="13"/>
       <c r="H19" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="6" t="s">
@@ -1508,22 +1620,22 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
     </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
       <c r="G20" s="13"/>
       <c r="H20" s="22" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="6" t="s">
@@ -1532,22 +1644,22 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
     </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="10"/>
       <c r="F21" s="6"/>
       <c r="G21" s="13"/>
       <c r="H21" s="22" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="6" t="s">
@@ -1556,22 +1668,24 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
     </row>
-    <row r="22" spans="1:12" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="G22" s="13"/>
       <c r="H22" s="22" t="s">
-        <v>93</v>
+        <v>148</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="6" t="s">
@@ -1580,22 +1694,22 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
     </row>
-    <row r="23" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="10"/>
       <c r="F23" s="6"/>
       <c r="G23" s="13"/>
       <c r="H23" s="22" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="6" t="s">
@@ -1604,22 +1718,22 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
     </row>
-    <row r="24" spans="1:12" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
       <c r="G24" s="13"/>
       <c r="H24" s="22" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="6" t="s">
@@ -1628,90 +1742,213 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
     </row>
-    <row r="25" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="10"/>
+      <c r="H25" s="22" t="s">
+        <v>89</v>
+      </c>
       <c r="I25" s="10"/>
-      <c r="J25" s="6"/>
+      <c r="J25" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
     </row>
-    <row r="26" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="9"/>
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
       <c r="F26" s="6"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="10"/>
+      <c r="H26" s="22" t="s">
+        <v>89</v>
+      </c>
       <c r="I26" s="10"/>
-      <c r="J26" s="6"/>
+      <c r="J26" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
     </row>
-    <row r="27" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I27" s="10"/>
+      <c r="J27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="J29" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+    </row>
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+    </row>
+    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="37"/>
+    </row>
+    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="B32" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
+      <c r="B33" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1724,7 +1961,7 @@
   <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1757,7 +1994,7 @@
     </row>
     <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>19</v>
@@ -1771,7 +2008,7 @@
     </row>
     <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>20</v>
@@ -1785,13 +2022,13 @@
     </row>
     <row r="4" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>40</v>
-      </c>
       <c r="C4" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -1799,13 +2036,13 @@
     </row>
     <row r="5" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -1813,7 +2050,7 @@
     </row>
     <row r="6" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>19</v>
@@ -1827,7 +2064,7 @@
     </row>
     <row r="7" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>20</v>
@@ -1841,13 +2078,13 @@
     </row>
     <row r="8" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
@@ -1855,13 +2092,13 @@
     </row>
     <row r="9" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
@@ -1869,13 +2106,13 @@
     </row>
     <row r="10" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -1883,13 +2120,13 @@
     </row>
     <row r="11" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>60</v>
-      </c>
       <c r="C11" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
@@ -1897,13 +2134,13 @@
     </row>
     <row r="12" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
@@ -1911,13 +2148,13 @@
     </row>
     <row r="13" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
@@ -1925,13 +2162,13 @@
     </row>
     <row r="14" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -1939,13 +2176,13 @@
     </row>
     <row r="15" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -1953,13 +2190,13 @@
     </row>
     <row r="16" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
@@ -1967,13 +2204,13 @@
     </row>
     <row r="17" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
@@ -1981,13 +2218,13 @@
     </row>
     <row r="18" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -1995,13 +2232,13 @@
     </row>
     <row r="19" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -2009,13 +2246,13 @@
     </row>
     <row r="20" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -2023,13 +2260,13 @@
     </row>
     <row r="21" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -2037,13 +2274,13 @@
     </row>
     <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -2051,13 +2288,13 @@
     </row>
     <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -2065,13 +2302,13 @@
     </row>
     <row r="24" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -2079,13 +2316,13 @@
     </row>
     <row r="25" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -2093,13 +2330,13 @@
     </row>
     <row r="26" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -2107,13 +2344,13 @@
     </row>
     <row r="27" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -2121,13 +2358,13 @@
     </row>
     <row r="28" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -2135,13 +2372,13 @@
     </row>
     <row r="29" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -2149,13 +2386,13 @@
     </row>
     <row r="30" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
@@ -2163,13 +2400,13 @@
     </row>
     <row r="31" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
@@ -2177,13 +2414,13 @@
     </row>
     <row r="32" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
@@ -2191,13 +2428,13 @@
     </row>
     <row r="33" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
@@ -2205,13 +2442,13 @@
     </row>
     <row r="34" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
@@ -2219,13 +2456,13 @@
     </row>
     <row r="35" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
@@ -2233,13 +2470,13 @@
     </row>
     <row r="36" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
@@ -2247,13 +2484,13 @@
     </row>
     <row r="37" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
@@ -2261,13 +2498,13 @@
     </row>
     <row r="38" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
@@ -2275,13 +2512,13 @@
     </row>
     <row r="39" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
@@ -2289,13 +2526,13 @@
     </row>
     <row r="40" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>138</v>
-      </c>
       <c r="C40" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
@@ -2303,13 +2540,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20"/>
@@ -2317,13 +2554,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
@@ -2331,13 +2568,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
@@ -2345,13 +2582,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
@@ -2359,13 +2596,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20"/>
@@ -2373,13 +2610,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
@@ -2387,13 +2624,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
@@ -2401,13 +2638,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
@@ -2415,13 +2652,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
@@ -2601,8 +2838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2627,10 +2864,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>

</xml_diff>